<commit_message>
Creazione RAM, modifica RACI
</commit_message>
<xml_diff>
--- a/Fase_2/RAM.xlsx
+++ b/Fase_2/RAM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\vscode\progetto gestione\GestioneProgetti\Fase_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Git\GestioneProgetti\Fase_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{328ABF27-9A01-4F07-9676-02796D8A2C1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6179C303-D384-4AA8-8C0F-809EB8284C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{8C7292EA-DD0F-4DBF-98E6-C9BD06E3E03B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8C7292EA-DD0F-4DBF-98E6-C9BD06E3E03B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="61">
   <si>
     <t>1.1 Definizione degli obiettivi del progetto</t>
   </si>
@@ -207,25 +207,7 @@
     <t>Piacentini Alessandro</t>
   </si>
   <si>
-    <t>Stakeholders</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>R/A</t>
-  </si>
-  <si>
-    <t>A/C</t>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -281,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9914445C-CD02-4581-B140-F9EDBB427865}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,1005 +611,805 @@
       <c r="E1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="D35" s="3"/>
       <c r="E35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B38" s="3"/>
       <c r="C38" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
-      <c r="F38" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B41" s="3"/>
       <c r="C41" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E41" s="3"/>
-      <c r="F41" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E47" s="3"/>
-      <c r="F47" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B48" s="3"/>
       <c r="C48" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B49" s="3"/>
       <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="D49" s="3"/>
       <c r="E49" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="B50" s="3"/>
       <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="D50" s="3"/>
       <c r="E50" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E53" s="3"/>
-      <c r="F53" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B54" s="3"/>
       <c r="C54" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E55" s="3"/>
-      <c r="F55" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="B56" s="3"/>
       <c r="C56" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>61</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
RAM aggiunti totali e corretto secondo indicazioni prof
</commit_message>
<xml_diff>
--- a/Fase_2/RAM.xlsx
+++ b/Fase_2/RAM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utente/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612B466F-AB6A-2D4F-AC95-6238CBD8F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399EF171-BEA6-1D43-BAC2-4F8EEDB5A518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{8C7292EA-DD0F-4DBF-98E6-C9BD06E3E03B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15200" windowHeight="15720" xr2:uid="{8C7292EA-DD0F-4DBF-98E6-C9BD06E3E03B}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
   <si>
     <t>1.1 Definizione degli obiettivi del progetto</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Totale</t>
   </si>
 </sst>
 </file>
@@ -270,7 +273,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -330,11 +333,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,10 +396,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -361,13 +411,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -684,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9914445C-CD02-4581-B140-F9EDBB427865}">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -711,42 +779,42 @@
       <c r="D1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -757,8 +825,8 @@
         <v>60</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -769,8 +837,8 @@
       <c r="D6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -779,10 +847,10 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="3"/>
+      <c r="E7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -793,8 +861,8 @@
         <v>60</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -803,10 +871,10 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="3"/>
+      <c r="E9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -815,8 +883,8 @@
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -827,8 +895,8 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -839,8 +907,8 @@
       <c r="D12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -851,8 +919,8 @@
         <v>60</v>
       </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -863,8 +931,8 @@
       <c r="D14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -873,10 +941,10 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="3"/>
+      <c r="E15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -887,8 +955,8 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -897,10 +965,10 @@
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="3"/>
+      <c r="E17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -909,30 +977,30 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="9"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -943,8 +1011,8 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -952,11 +1020,11 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="D22" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -964,9 +1032,9 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -977,8 +1045,8 @@
         <v>60</v>
       </c>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -987,10 +1055,10 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="3"/>
+      <c r="E25" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
@@ -999,8 +1067,8 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="3"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -1011,40 +1079,40 @@
       <c r="D27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="11"/>
+      <c r="B29" s="7"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
@@ -1055,8 +1123,8 @@
         <v>60</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="19"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
@@ -1067,8 +1135,8 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
@@ -1079,8 +1147,8 @@
       <c r="D33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="19"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
@@ -1091,8 +1159,8 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
@@ -1101,10 +1169,10 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="3"/>
+      <c r="E35" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="19"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
@@ -1113,8 +1181,8 @@
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="3"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
@@ -1123,8 +1191,8 @@
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -1135,30 +1203,30 @@
         <v>60</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="19"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="9"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
@@ -1169,8 +1237,8 @@
         <v>60</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="19"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -1181,40 +1249,40 @@
       <c r="D42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B43" s="3"/>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="6" t="s">
         <v>60</v>
       </c>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="19"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="3"/>
-      <c r="C44" s="11"/>
+      <c r="C44" s="7"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="3"/>
-      <c r="C45" s="12"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="19"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
@@ -1222,11 +1290,11 @@
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
-      <c r="D46" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="D46" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -1234,9 +1302,9 @@
       </c>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="19"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
@@ -1247,8 +1315,8 @@
         <v>60</v>
       </c>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="19"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
@@ -1257,10 +1325,10 @@
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="3"/>
+      <c r="E49" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
@@ -1269,8 +1337,8 @@
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="3"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="19"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
@@ -1281,8 +1349,8 @@
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="19"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
@@ -1293,8 +1361,8 @@
       <c r="D52" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="19"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
@@ -1303,8 +1371,8 @@
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
@@ -1313,10 +1381,10 @@
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F54" s="3"/>
+      <c r="E54" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F54" s="19"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
@@ -1325,8 +1393,8 @@
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
@@ -1337,8 +1405,8 @@
         <v>60</v>
       </c>
       <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="19"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
@@ -1349,29 +1417,45 @@
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="19"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B58">
+      <c r="B58" s="2">
         <f>COUNTIF(B2:B57,"x")</f>
         <v>10</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="2">
         <f>COUNTIF(C2:C57,"x")</f>
         <v>11</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="2">
         <f>COUNTIF(D2:D57,"x")</f>
         <v>9</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <f>COUNTIF(E2:E57,"x")</f>
         <v>8</v>
       </c>
+      <c r="F58" s="19"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C60" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="2">
+        <f>SUM(B58:E58)</f>
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D22:D23"/>
     <mergeCell ref="D52:D53"/>
     <mergeCell ref="E54:E55"/>
     <mergeCell ref="B28:B30"/>
@@ -1380,12 +1464,6 @@
     <mergeCell ref="C43:C45"/>
     <mergeCell ref="D46:D47"/>
     <mergeCell ref="E49:E50"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E25:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>